<commit_message>
BOM v 0.5 updated
</commit_message>
<xml_diff>
--- a/System_development/Jocassee/V0.5.0/BIll_Of_Matirials/Water quality V0.5 BOM.xlsx
+++ b/System_development/Jocassee/V0.5.0/BIll_Of_Matirials/Water quality V0.5 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailsc-my.sharepoint.com/personal/asifuzzaman_sc_edu/Documents/Github Repos/In-Situ-Water-Quality-Sensor/System_development/Jocassee/V0.5.0/BIll_Of_Matirials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:1_{6B961E68-D31B-4521-91FF-D3DA3F24FD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77A748BC-657C-4C6A-B3C3-DB990EDD4CA7}"/>
+  <xr:revisionPtr revIDLastSave="269" documentId="13_ncr:1_{6B961E68-D31B-4521-91FF-D3DA3F24FD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9544215C-83FB-454B-A8F8-1E2626C8473F}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{3F872AE6-6710-4898-8598-9832416C0361}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3F872AE6-6710-4898-8598-9832416C0361}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics BOM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
   <si>
     <t>Qty</t>
   </si>
@@ -54,181 +54,217 @@
     <t>U8</t>
   </si>
   <si>
+    <t>PCB Reference</t>
+  </si>
+  <si>
+    <t>Unit cost (USD)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Net cost (USD)</t>
+  </si>
+  <si>
+    <t>Vendor 1</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_1206_3216Metric_Pad1.33x1.80mm_HandSolder</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_1206_3216Metric_Pad1.30x1.75mm_HandSolder</t>
+  </si>
+  <si>
+    <t>SD card module</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Arduino Nano</t>
+  </si>
+  <si>
+    <t>DS3231M</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>C1 0.1uF</t>
+  </si>
+  <si>
+    <t>R2 470ohm</t>
+  </si>
+  <si>
+    <t>3pin XH2.54 male connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-XH-A/1651046</t>
+  </si>
+  <si>
+    <t>R1 4.7K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/atlas-scientific/SRV-PH/16003016?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLlgG2JWtg72d3seRm9FjQrAou&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hznU8J98oZ-_7GD7xu8VgPNOpSYHGji59g_m7GB07rUIyNC8TPEMLYhoCYgIQAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>Atlas pH conditioning circuit</t>
+  </si>
+  <si>
+    <t>ds18b20 temperature sensor</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/atlas-scientific/ENV-30-PH/16003028?gad_source=1&amp;gad_campaignid=20232005509&amp;gbraid=0AAAAADrbLliv6K8bW91YgzNqrt8ONo2QZ&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzpcO_PthZYBVBiTP7blHnIK4NnAfIL94wP-XbBh0unyx4OZTtFbw-hoC7p4QAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>11.1V 3300mAH Lipo battery with T connector</t>
+  </si>
+  <si>
+    <t>Male T connector for lipo</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nextgen-components/1206B104K500BD/15776047?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbRACYBmADgHYaQBdAgBwBcoQBlNgJwEsAdgHMQAXwLkADLACcCEMkjps%2BIqRBSAdGAAEAVoBiTVh0ggAqoP5sA8igCyONFgCuvHOIIBaeNEWomLgExJBkAGyUAKxRTGISFBqIaCxoiDaEvHFAA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/151033RS03000/4490003</t>
+  </si>
+  <si>
+    <t>15 pin female header 2.54 mm</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/11864/6818769?gad_source=1&amp;gad_campaignid=20470400566&amp;gbraid=0AAAAADrbLliIHIRZTdCUnz0dgTjq27lO9&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzmI8CZGH_aIaTxCITd4vJTEk9RuU9JLQrgEuPZd__e3-SqyQUR2pSRoCVAQQAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/203852249807?_skw=SD+card+module+mini&amp;itmmeta=01JWS7YRSNYRE9JPQ1403XF1SB&amp;hash=item2f768a7acf:g:8QAAAOSwqApl32li&amp;itmprp=enc%3AAQAKAAAA8FkggFvd1GGDu0w3yXCmi1ebfwHB6lyAy277lL4U8xOIhySGOtjI0bRPLZxMt0nwv62q7s0aZTz%2Bx%2F%2B7upL3MEA0K%2Ft0uJJWEl1PUNUul0C2kuW4nvX2%2BRwcD%2FhFGnTe%2FYG8zjgNvBu3TQY4IOsJphAfcfdUNAqbhaX7gXxY59Lj77JBWoN7w1LfwWyMjbSTm6GobMFWOs8mooWe2dthd87YxK7TTSBoyUD9D2pQE62PZubKATklktRZLCgMHdh0lcqvJRpnSkfD1qwChuyoZk51pvBJMF9jfr6RlQAGIR8TsCDyF0H7ZR59sGEcWXB%2FYA%3D%3D%7Ctkp%3ABFBMhI37p-Zl</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/283932038203?_skw=arduino+nano&amp;itmmeta=01JWS81PY2BK5W7AA2FK7T4DBS&amp;hash=item421bab143b:g:LEAAAOSwdsFg2bYB&amp;itmprp=enc%3AAQAKAAAA8FkggFvd1GGDu0w3yXCmi1ctIY2mddW3r0Pkz46AoULbxKR%2BLiu5WOk62feEjacXqpl7sNYJ6oE5%2FIn8lx78btygJOm2GvQyRb5jvCpCuuGSTVPm9c07lGI3HNmnry6uXc%2FlnST9gzmAQ3twOlrPRg6L2z%2FrDEBP6lCqIj7RU29pAxunTYC5VGu28NSWzm60eskDXI6rlTmkwJlAt4v66kpFByyhd4g%2F6NwsaYSfKxSXG6ADA884XQD96VOVCodbJCGKGFFk37cKyzrKEAETZC68GmzoBgXTDf9gi8GNs2wRWd%2FEf3cay51rfG1Vttxmiw%3D%3D%7Ctkp%3ABk9SR5jvhqjmZQ</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/DS3231M-TRL/2402421</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/mpd-memory-protection-devices/BK-870/3829737</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR1206-JW-471ELF/3741054</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR1206-JW-472ELF/3785627</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jauch-quartz/CR1025/16399048</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/184291373846?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=184291373846&amp;targetid=2299003535955&amp;device=c&amp;mktype=pla&amp;googleloc=9010352&amp;poi=&amp;campaignid=21214315381&amp;mkgroupid=161363866036&amp;rlsatarget=pla-2299003535955&amp;abcId=9407526&amp;merchantid=114832125&amp;gad_source=1&amp;gad_campaignid=21214315381&amp;gbraid=0AAAAAD_QDh-WxDW3V6tycLWe8cGWhVCet&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzg3Q1Yr5Qywajf85ozukT0eBrnuBw2qcSHroRC1sgV2p7BH7wwA-ZRoCue8QAvD_BwE</t>
+  </si>
+  <si>
+    <t>TDS probe and conditioning circuit</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/224193475936?_skw=ds18b20&amp;itmmeta=01JWS9436Y9FERAQTKDM3HA2HJ&amp;hash=item3432f8f560:g:o3YAAOSwU~BfhkxY&amp;itmprp=enc%3AAQAKAAAA4FkggFvd1GGDu0w3yXCmi1eZVpkWHqnJ1CXCxYwe7hH8MTDd21uDFcQkxB6UmuFL1nzEvMyPnwrLbfpibrtSw6PJ6oEOTjHA%2BkjlTR3A1QaHWZf0kE2w%2FhydudbtDkwEMazkGGG3RxFLdxOnAGzZBTlCUEFESqTvAhNn%2Bjye4iJMlnnPGLOgNL40CCfjp7qUswlfOwv0yjnO%2Ft2tQ0Gx2dXExLjwUsFFwJLjU6q8t9vdK3%2FxrsrClja0ZOKas2024SmxIkA1w06CzLtlKOw3UkAT%2B%2FRsayZchEvbfvz6zTfc%7Ctkp%3ABFBM0rOQqeZl</t>
+  </si>
+  <si>
+    <t>Vendor 2</t>
+  </si>
+  <si>
+    <t>Vendor 3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/SSW-115-01-F-S/7879494?gad_source=1&amp;gad_campaignid=17336967819&amp;gbraid=0AAAAADrbLlhPPMEXoJVxfpFdpEMhcu0YV&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66X6luvpzic7SpeQdTZEq5PP26iV0Bmu3w1zSQ-hOKFa4-GjmDPOJZMaAjkJEALw_wcB&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/c-k/OS102011MS2QN1/411602</t>
+  </si>
+  <si>
+    <t>SWITCH OS102011MS2QN1</t>
+  </si>
+  <si>
+    <t>LED 3.0mm</t>
+  </si>
+  <si>
+    <t>Coin cell battery CR-1025-ND</t>
+  </si>
+  <si>
+    <t>Coin cell Battery Holder BK-870</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/dfrobot/SEN0189/6588606?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLljucuLmqEe4bIBP9pEZ4VG5H&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66VOazEoiMlVT5LyfIrJo00cvNuFdGVQSUgYSB1oL8UVePiNsSg_drQaAosTEALw_wcB&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>Component spec / part number</t>
+  </si>
+  <si>
+    <t>PCB itself</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/</t>
+  </si>
+  <si>
+    <t>https://www.keyestudio.com/products/keyestudio-turbidity-sensor-v10-with-wires-compatible-with-arduino-for-water-testing</t>
+  </si>
+  <si>
+    <t>Turbidity conditioning circuit and sensor</t>
+  </si>
+  <si>
+    <t>pH probe ENV 30</t>
+  </si>
+  <si>
+    <t>https://atlas-scientific.com/probes/consumer-grade-ph-probe/?srsltid=AfmBOoog-hWZh-AcQq7td_rVXcdNzJnbRIhdNeb6Zga2Xtm4j7G4n8_-</t>
+  </si>
+  <si>
+    <t>https://www.keyestudio.com/products/keyestudio-tds-meter-v10-board-module-water-meter-filter-measuring-water-quality-for-arduino-unor3</t>
+  </si>
+  <si>
     <t>Component</t>
   </si>
   <si>
-    <t>PCB Reference</t>
-  </si>
-  <si>
-    <t>Unit cost (USD)</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Net cost (USD)</t>
+    <t xml:space="preserve">Qty per sensor </t>
+  </si>
+  <si>
+    <t>vendor 1</t>
+  </si>
+  <si>
+    <t>vendor 2</t>
+  </si>
+  <si>
+    <t>vendor 3</t>
   </si>
   <si>
     <t>PVC union</t>
   </si>
   <si>
-    <t>1 ft</t>
-  </si>
-  <si>
-    <t>vendor 1</t>
-  </si>
-  <si>
     <t>https://www.grainger.com/product/22FL17?RIID=51819294775&amp;GID=729415832&amp;mid=OrderConfirmation_REST&amp;rfe=d3a2685b7c662b4e6de9ad0036b442e97d0be97efaa150f15a85f91dfbe56413&amp;gucid=EMT:11126144:Item:CSM-323&amp;emcid=NA:Item</t>
   </si>
   <si>
+    <t>Schedule 40 clear PVC pipe</t>
+  </si>
+  <si>
+    <t>10 inches</t>
+  </si>
+  <si>
     <t>https://www.grainger.com/product/1AAZ8?RIID=51819294775&amp;GID=729415832&amp;mid=OrderConfirmation_REST&amp;rfe=d3a2685b7c662b4e6de9ad0036b442e97d0be97efaa150f15a85f91dfbe56413&amp;gucid=EMT:11126144:Item:CSM-323&amp;emcid=NA:Item</t>
   </si>
   <si>
     <t>Schedule 40 socket cap</t>
   </si>
   <si>
-    <t>vendor 2</t>
-  </si>
-  <si>
-    <t>Vendor 1</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_1206_3216Metric_Pad1.33x1.80mm_HandSolder</t>
-  </si>
-  <si>
-    <t>Resistor_SMD:R_1206_3216Metric_Pad1.30x1.75mm_HandSolder</t>
-  </si>
-  <si>
-    <t>SD card module</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>Arduino Nano</t>
-  </si>
-  <si>
-    <t>DS3231M</t>
-  </si>
-  <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>C1 0.1uF</t>
-  </si>
-  <si>
-    <t>R2 470ohm</t>
-  </si>
-  <si>
-    <t>3pin XH2.54 male connector</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-XH-A/1651046</t>
-  </si>
-  <si>
-    <t>R1 4.7K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/atlas-scientific/SRV-PH/16003016?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLlgG2JWtg72d3seRm9FjQrAou&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hznU8J98oZ-_7GD7xu8VgPNOpSYHGji59g_m7GB07rUIyNC8TPEMLYhoCYgIQAvD_BwE&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>Atlas pH conditioning circuit</t>
-  </si>
-  <si>
-    <t>pH probe</t>
-  </si>
-  <si>
-    <t>ds18b20 temperature sensor</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/atlas-scientific/ENV-30-PH/16003028?gad_source=1&amp;gad_campaignid=20232005509&amp;gbraid=0AAAAADrbLliv6K8bW91YgzNqrt8ONo2QZ&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzpcO_PthZYBVBiTP7blHnIK4NnAfIL94wP-XbBh0unyx4OZTtFbw-hoC7p4QAvD_BwE&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>11.1V 3300mAH Lipo battery with T connector</t>
-  </si>
-  <si>
-    <t>Male T connector for lipo</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/nextgen-components/1206B104K500BD/15776047?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbRACYBmADgHYaQBdAgBwBcoQBlNgJwEsAdgHMQAXwLkADLACcCEMkjps%2BIqRBSAdGAAEAVoBiTVh0ggAqoP5sA8igCyONFgCuvHOIIBaeNEWomLgExJBkAGyUAKxRTGISFBqIaCxoiDaEvHFAA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/151033RS03000/4490003</t>
-  </si>
-  <si>
-    <t>15 pin female header 2.54 mm</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/11864/6818769?gad_source=1&amp;gad_campaignid=20470400566&amp;gbraid=0AAAAADrbLliIHIRZTdCUnz0dgTjq27lO9&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzmI8CZGH_aIaTxCITd4vJTEk9RuU9JLQrgEuPZd__e3-SqyQUR2pSRoCVAQQAvD_BwE&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/203852249807?_skw=SD+card+module+mini&amp;itmmeta=01JWS7YRSNYRE9JPQ1403XF1SB&amp;hash=item2f768a7acf:g:8QAAAOSwqApl32li&amp;itmprp=enc%3AAQAKAAAA8FkggFvd1GGDu0w3yXCmi1ebfwHB6lyAy277lL4U8xOIhySGOtjI0bRPLZxMt0nwv62q7s0aZTz%2Bx%2F%2B7upL3MEA0K%2Ft0uJJWEl1PUNUul0C2kuW4nvX2%2BRwcD%2FhFGnTe%2FYG8zjgNvBu3TQY4IOsJphAfcfdUNAqbhaX7gXxY59Lj77JBWoN7w1LfwWyMjbSTm6GobMFWOs8mooWe2dthd87YxK7TTSBoyUD9D2pQE62PZubKATklktRZLCgMHdh0lcqvJRpnSkfD1qwChuyoZk51pvBJMF9jfr6RlQAGIR8TsCDyF0H7ZR59sGEcWXB%2FYA%3D%3D%7Ctkp%3ABFBMhI37p-Zl</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/283932038203?_skw=arduino+nano&amp;itmmeta=01JWS81PY2BK5W7AA2FK7T4DBS&amp;hash=item421bab143b:g:LEAAAOSwdsFg2bYB&amp;itmprp=enc%3AAQAKAAAA8FkggFvd1GGDu0w3yXCmi1ctIY2mddW3r0Pkz46AoULbxKR%2BLiu5WOk62feEjacXqpl7sNYJ6oE5%2FIn8lx78btygJOm2GvQyRb5jvCpCuuGSTVPm9c07lGI3HNmnry6uXc%2FlnST9gzmAQ3twOlrPRg6L2z%2FrDEBP6lCqIj7RU29pAxunTYC5VGu28NSWzm60eskDXI6rlTmkwJlAt4v66kpFByyhd4g%2F6NwsaYSfKxSXG6ADA884XQD96VOVCodbJCGKGFFk37cKyzrKEAETZC68GmzoBgXTDf9gi8GNs2wRWd%2FEf3cay51rfG1Vttxmiw%3D%3D%7Ctkp%3ABk9SR5jvhqjmZQ</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/DS3231M-TRL/2402421</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/mpd-memory-protection-devices/BK-870/3829737</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR1206-JW-471ELF/3741054</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR1206-JW-472ELF/3785627</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/jauch-quartz/CR1025/16399048</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/184291373846?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=184291373846&amp;targetid=2299003535955&amp;device=c&amp;mktype=pla&amp;googleloc=9010352&amp;poi=&amp;campaignid=21214315381&amp;mkgroupid=161363866036&amp;rlsatarget=pla-2299003535955&amp;abcId=9407526&amp;merchantid=114832125&amp;gad_source=1&amp;gad_campaignid=21214315381&amp;gbraid=0AAAAAD_QDh-WxDW3V6tycLWe8cGWhVCet&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzg3Q1Yr5Qywajf85ozukT0eBrnuBw2qcSHroRC1sgV2p7BH7wwA-ZRoCue8QAvD_BwE</t>
-  </si>
-  <si>
-    <t>TDS probe and conditioning circuit</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/224193475936?_skw=ds18b20&amp;itmmeta=01JWS9436Y9FERAQTKDM3HA2HJ&amp;hash=item3432f8f560:g:o3YAAOSwU~BfhkxY&amp;itmprp=enc%3AAQAKAAAA4FkggFvd1GGDu0w3yXCmi1eZVpkWHqnJ1CXCxYwe7hH8MTDd21uDFcQkxB6UmuFL1nzEvMyPnwrLbfpibrtSw6PJ6oEOTjHA%2BkjlTR3A1QaHWZf0kE2w%2FhydudbtDkwEMazkGGG3RxFLdxOnAGzZBTlCUEFESqTvAhNn%2Bjye4iJMlnnPGLOgNL40CCfjp7qUswlfOwv0yjnO%2Ft2tQ0Gx2dXExLjwUsFFwJLjU6q8t9vdK3%2FxrsrClja0ZOKas2024SmxIkA1w06CzLtlKOw3UkAT%2B%2FRsayZchEvbfvz6zTfc%7Ctkp%3ABFBM0rOQqeZl</t>
-  </si>
-  <si>
-    <t>Vendor 2</t>
-  </si>
-  <si>
-    <t>Vendor 3</t>
-  </si>
-  <si>
-    <t>vendor 3</t>
-  </si>
-  <si>
-    <t>Schedule 40 clear PVC pipe</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/samtec-inc/SSW-115-01-F-S/7879494?gad_source=1&amp;gad_campaignid=17336967819&amp;gbraid=0AAAAADrbLlhPPMEXoJVxfpFdpEMhcu0YV&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66X6luvpzic7SpeQdTZEq5PP26iV0Bmu3w1zSQ-hOKFa4-GjmDPOJZMaAjkJEALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/c-k/OS102011MS2QN1/411602</t>
-  </si>
-  <si>
-    <t>SWITCH OS102011MS2QN1</t>
-  </si>
-  <si>
-    <t>LED 3.0mm</t>
-  </si>
-  <si>
-    <t>Coin cell battery CR-1025-ND</t>
-  </si>
-  <si>
-    <t>Coin cell Battery Holder BK-870</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/dfrobot/SEN0189/6588606?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLljucuLmqEe4bIBP9pEZ4VG5H&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66VOazEoiMlVT5LyfIrJo00cvNuFdGVQSUgYSB1oL8UVePiNsSg_drQaAosTEALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>DF robot Turbidity conditioning circuit and sensor</t>
+    <t>2 part epoxy</t>
+  </si>
+  <si>
+    <t>Net price (USD)</t>
+  </si>
+  <si>
+    <t>Unit price (USD)</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/25F529?gucid=N:N:PS:Paid:GGL:CSM-2295:7Q8R4W:20500801:APZ_1&amp;gad_source=1&amp;gad_campaignid=21369464154&amp;gclid=CjwKCAjwr5_CBhBlEiwAzfwYuFQJQF4xih2fA0vbI8pFLV_pGSsb1GvVdYQqLORI5ApakqFVLNHuxxoCPr8QAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>1 pack</t>
   </si>
 </sst>
 </file>
@@ -392,7 +428,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,8 +620,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -726,6 +768,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -772,7 +836,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -780,15 +844,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -799,12 +893,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -813,26 +904,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1214,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF72E9-9057-43B3-9849-7848ED564DB8}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1232,380 +1311,408 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="12"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="21">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="21">
-        <v>1</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="21">
-        <v>1</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="21">
-        <v>1</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="21">
-        <v>1</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="21">
-        <v>1</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="21">
-        <v>1</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="21">
-        <v>1</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="21">
-        <v>1</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="21">
-        <v>1</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="21">
-        <v>1</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="21">
-        <v>1</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="21">
-        <v>1</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="21">
-        <v>1</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="21">
-        <v>1</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="21">
-        <v>1</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="21">
-        <v>1</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="21">
-        <v>1</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="21">
-        <v>2</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="6">
+      <c r="E22" s="14">
         <f>SUM(E2:E20)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1628,129 +1735,130 @@
     <hyperlink ref="F18" r:id="rId17" display="https://www.ebay.com/itm/224193475936?_skw=ds18b20&amp;itmmeta=01JWS9436Y9FERAQTKDM3HA2HJ&amp;hash=item3432f8f560:g:o3YAAOSwU~BfhkxY&amp;itmprp=enc%3AAQAKAAAA4FkggFvd1GGDu0w3yXCmi1eZVpkWHqnJ1CXCxYwe7hH8MTDd21uDFcQkxB6UmuFL1nzEvMyPnwrLbfpibrtSw6PJ6oEOTjHA%2BkjlTR3A1QaHWZf0kE2w%2FhydudbtDkwEMazkGGG3RxFLdxOnAGzZBTlCUEFESqTvAhNn%2Bjye4iJMlnnPGLOgNL40CCfjp7qUswlfOwv0yjnO%2Ft2tQ0Gx2dXExLjwUsFFwJLjU6q8t9vdK3%2FxrsrClja0ZOKas2024SmxIkA1w06CzLtlKOw3UkAT%2B%2FRsayZchEvbfvz6zTfc%7Ctkp%3ABFBM0rOQqeZl" xr:uid="{6CE59FE4-3B5B-463E-8BFA-AE84C9657E1C}"/>
     <hyperlink ref="F20" r:id="rId18" display="https://www.digikey.com/en/products/detail/samtec-inc/SSW-115-01-F-S/7879494?gad_source=1&amp;gad_campaignid=17336967819&amp;gbraid=0AAAAADrbLlhPPMEXoJVxfpFdpEMhcu0YV&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66X6luvpzic7SpeQdTZEq5PP26iV0Bmu3w1zSQ-hOKFa4-GjmDPOJZMaAjkJEALw_wcB&amp;gclsrc=aw.ds" xr:uid="{9B3BC39D-EF5B-4388-80DC-969E3750D113}"/>
     <hyperlink ref="F3" r:id="rId19" xr:uid="{9557BBDE-7B36-4980-B2CF-6CC83594058E}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{5DC5AA7A-D293-4D8B-BD8A-6D666E0FFFDC}"/>
+    <hyperlink ref="G15" r:id="rId21" xr:uid="{6C5CD10F-CC8B-41D0-AFD8-4F3D53674579}"/>
+    <hyperlink ref="G16" r:id="rId22" xr:uid="{7CCAC606-6D69-4384-A632-81B17260CDA3}"/>
+    <hyperlink ref="G17" r:id="rId23" xr:uid="{4C6031E9-5DB5-420D-A786-DB2505BC5E3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FC38E1-F200-4776-BB4D-C01A4F63E4E3}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC825CFC-606A-4EB1-BF18-3BEFDFC7363F}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.36328125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="7.90625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="56.7265625" style="10" customWidth="1"/>
-    <col min="6" max="7" width="58" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="10"/>
+    <col min="1" max="1" width="35.36328125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" style="22" customWidth="1"/>
+    <col min="3" max="4" width="18.81640625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="65.453125" style="18" customWidth="1"/>
+    <col min="6" max="7" width="58" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="11">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12">
-        <v>19.55</v>
-      </c>
-      <c r="D2" s="12">
-        <f>PRODUCT(B2,C2)</f>
-        <v>19.55</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="A1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="12">
-        <v>7.9</v>
-      </c>
-      <c r="D3" s="12">
-        <f t="shared" ref="D3:D4" si="0">PRODUCT(B3,C3)</f>
-        <v>7.9</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="A3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="11">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12">
-        <v>0.78</v>
-      </c>
-      <c r="D4" s="12">
-        <f t="shared" si="0"/>
-        <v>0.78</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="17">
-        <f>SUM(D2:D4)</f>
-        <v>28.230000000000004</v>
-      </c>
-      <c r="E5" s="13"/>
+      <c r="A4" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="23">
+        <v>47.86</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{0ADC6640-CDF3-43BB-8CD8-72CCE1972888}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{C3E7FD7D-6E84-411F-9543-A725D0E138A2}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{397E3EDA-4EB7-4A45-BAD0-12FFD4DA64AA}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{A96C4A01-B17D-4787-93F2-14FC70C6E519}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{9A0D2115-F482-46FE-A053-05FBD455939B}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{4B7D939A-3AAC-42AA-8866-337F66719F37}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{BB44769E-9C2A-4FEF-A4D5-DBD7D743C569}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code and BOM updated
</commit_message>
<xml_diff>
--- a/System_development/Jocassee/V0.5.0/BIll_Of_Matirials/Water quality V0.5 BOM.xlsx
+++ b/System_development/Jocassee/V0.5.0/BIll_Of_Matirials/Water quality V0.5 BOM.xlsx
@@ -2,22 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailsc-my.sharepoint.com/personal/asifuzzaman_sc_edu/Documents/Github Repos/In-Situ-Water-Quality-Sensor/System_development/Jocassee/V0.5.0/BIll_Of_Matirials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="300" documentId="13_ncr:1_{6B961E68-D31B-4521-91FF-D3DA3F24FD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44B82CCA-033D-4D40-9007-FB64776F859A}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{B25A7C33-3DB6-4E9E-AD5A-98A1F049AD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70AFA17C-64BC-4378-B771-CCB4BD04F536}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{3F872AE6-6710-4898-8598-9832416C0361}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3F872AE6-6710-4898-8598-9832416C0361}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics BOM" sheetId="1" r:id="rId1"/>
     <sheet name="Fixture BOM" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,197 +37,227 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
+  <si>
+    <t>PCB Reference</t>
+  </si>
+  <si>
+    <t>Component spec / part number</t>
+  </si>
   <si>
     <t>Qty</t>
   </si>
   <si>
+    <t>Unit cost (USD)</t>
+  </si>
+  <si>
+    <t>Net cost (USD)</t>
+  </si>
+  <si>
+    <t>Vendor 1</t>
+  </si>
+  <si>
+    <t>Vendor 2</t>
+  </si>
+  <si>
+    <t>Vendor 3</t>
+  </si>
+  <si>
+    <t>C1 0.1uF</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_1206_3216Metric_Pad1.33x1.80mm_HandSolder</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nextgen-components/1206B104K500BD/15776047?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbRACYBmADgHYaQBdAgBwBcoQBlNgJwEsAdgHMQAXwLkADLACcCEMkjps%2BIqRBSAdGAAEAVoBiTVh0ggAqoP5sA8igCyONFgCuvHOIIBaeNEWomLgExJBkAGyUAKxRTGISFBqIaCxoiDaEvHFAA</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SWITCH OS102011MS2QN1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/c-k/OS102011MS2QN1/411602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/CK/OS102011MS2QN1?qs=WtljUlYws5RvQ1hEv876nQ%3D%3D&amp;mgh=1&amp;utm_id=22174357374&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_marketing_tactic=amercorp&amp;gad_source=1&amp;gad_campaignid=22295195434&amp;gbraid=0AAAAADn_wf37NcPripZZCoy9AiD-OvAcG&amp;gclid=Cj0KCQjwgvnCBhCqARIsADBLZoKyGA5ClHUZR7eCJ8ET8sUhF8oXtsBAC19VweIc1X0k5wSmKxZJZCcaAhNFEALw_wcB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jameco.com/z/OS102011MS2QN1-C-K-Slide-Switch-SPDT-ON-ON-100mA-12VDC-Through-Hole-5-08mm-Pitch_2313927.html?srsltid=AfmBOooPbd-Z6ToSODltkR-iIt2ROKqtFbsAIQSOobzGyu7T6KQzSeXa. </t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
+    <t>LED 3.0mm</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/151033RS03000/4490003</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
-    <t>U3</t>
+    <t>SD card module</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/203852249807?_skw=SD+card+module+mini&amp;itmmeta=01JWS7YRSNYRE9JPQ1403XF1SB&amp;hash=item2f768a7acf:g:8QAAAOSwqApl32li&amp;itmprp=enc%3AAQAKAAAA8FkggFvd1GGDu0w3yXCmi1ebfwHB6lyAy277lL4U8xOIhySGOtjI0bRPLZxMt0nwv62q7s0aZTz%2Bx%2F%2B7upL3MEA0K%2Ft0uJJWEl1PUNUul0C2kuW4nvX2%2BRwcD%2FhFGnTe%2FYG8zjgNvBu3TQY4IOsJphAfcfdUNAqbhaX7gXxY59Lj77JBWoN7w1LfwWyMjbSTm6GobMFWOs8mooWe2dthd87YxK7TTSBoyUD9D2pQE62PZubKATklktRZLCgMHdh0lcqvJRpnSkfD1qwChuyoZk51pvBJMF9jfr6RlQAGIR8TsCDyF0H7ZR59sGEcWXB%2FYA%3D%3D%7Ctkp%3ABFBMhI37p-Zl</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Arduino Nano</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/283932038203?_skw=arduino+nano&amp;itmmeta=01JWS81PY2BK5W7AA2FK7T4DBS&amp;hash=item421bab143b:g:LEAAAOSwdsFg2bYB&amp;itmprp=enc%3AAQAKAAAA8FkggFvd1GGDu0w3yXCmi1ctIY2mddW3r0Pkz46AoULbxKR%2BLiu5WOk62feEjacXqpl7sNYJ6oE5%2FIn8lx78btygJOm2GvQyRb5jvCpCuuGSTVPm9c07lGI3HNmnry6uXc%2FlnST9gzmAQ3twOlrPRg6L2z%2FrDEBP6lCqIj7RU29pAxunTYC5VGu28NSWzm60eskDXI6rlTmkwJlAt4v66kpFByyhd4g%2F6NwsaYSfKxSXG6ADA884XQD96VOVCodbJCGKGFFk37cKyzrKEAETZC68GmzoBgXTDf9gi8GNs2wRWd%2FEf3cay51rfG1Vttxmiw%3D%3D%7Ctkp%3ABk9SR5jvhqjmZQ</t>
   </si>
   <si>
     <t>U6</t>
   </si>
   <si>
+    <t>DS3231M+</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/DS3231M-TRL/2402421</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Analog-Devices-Maxim-Integrated/DS3231M+TRL?qs=Bakm8ERcljq5PBzSwLfmgg%3D%3D&amp;utm_id=22337522785&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_marketing_tactic=amercorp&amp;gad_source=1&amp;gad_campaignid=22327353774&amp;gbraid=0AAAAADn_wf3tXOv7c9Y4wq2-Yvx_HD5I2&amp;gclid=Cj0KCQjwgvnCBhCqARIsADBLZoJwmYFO86Wu0iC_hUhm8R9ynjb29I-YIssyZ4USDWwZGmZXPXlNSLQaAlaREALw_wcB</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>Coin cell Battery Holder BK-870</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/mpd-memory-protection-devices/BK-870/3829737</t>
+  </si>
+  <si>
     <t>U8</t>
   </si>
   <si>
-    <t>PCB Reference</t>
-  </si>
-  <si>
-    <t>Unit cost (USD)</t>
+    <t>3pin XH2.54 male connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-XH-A/1651046</t>
+  </si>
+  <si>
+    <t>R2 470ohm</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_1206_3216Metric_Pad1.30x1.75mm_HandSolder</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR1206-JW-471ELF/3741054</t>
+  </si>
+  <si>
+    <t>R1 4.7K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR1206-JW-472ELF/3785627</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Coin cell battery CR-1025-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jauch-quartz/CR1025/16399048</t>
+  </si>
+  <si>
+    <t>11.1V 3300mAH Lipo battery with T connector</t>
+  </si>
+  <si>
+    <t>https://us.ovonicshop.com/products/2-ovonic-3000mah-3s-50c-lipo-battery-11-1v-long-with-t-plug-for-aircraft?variant=49495640736024&amp;country=US&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;gad_source=1&amp;gad_campaignid=22231059484&amp;gbraid=0AAAAADH9voLksvZtdQfP_qv6g9D5uP4vz&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7wVC7linJpS4qPBFEeagS1am8YjtEL9eHuExf6EBj_sSKmwI5S25AaAmK1EALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/184508325888?chn=ps&amp;_trkparms=ispr%3D1&amp;amdata=enc%3A1ylpS771GTUqS6YST7-apLg15&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=184508325888&amp;targetid=2321110924221&amp;device=c&amp;mktype=pla&amp;googleloc=9010433&amp;poi=&amp;campaignid=21400684010&amp;mkgroupid=173029508068&amp;rlsatarget=aud-1317046432738:pla-2321110924221&amp;abcId=9448486&amp;merchantid=118955226&amp;gad_source=1&amp;gad_campaignid=21400684010&amp;gbraid=0AAAAAD_QDh99tBHCSfvM5L2BJj0mpS-rS&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7LhNJPcz_yB99-iNQOigF1uTLSpT72VMRZDt4bpaZcj-4-2mtZYDUaAlYNEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.motionrc.com/products/admiral-3300mah-3s-11-1v-30c-lipo-battery-with-t-connector-epr33003?variant=19047011142&amp;country=US&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;gad_source=1&amp;gad_campaignid=15448361688&amp;gbraid=0AAAAADrr98ZD1fBrj_NSKbi2hqFZgUrfk&amp;gclid=Cj0KCQjwgvnCBhCqARIsADBLZoIjaMcUy2YxUOv0QnymhbqBDrWMvbmN8Xkj10xanB3EhIRIsKdz-QAaAkkxEALw_wcB</t>
+  </si>
+  <si>
+    <t>Atlas pH conditioning circuit</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/atlas-scientific/SRV-PH/16003016?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLlgG2JWtg72d3seRm9FjQrAou&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hznU8J98oZ-_7GD7xu8VgPNOpSYHGji59g_m7GB07rUIyNC8TPEMLYhoCYgIQAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>Turbidity conditioning circuit and sensor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/dfrobot/SEN0189/6588606?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLljucuLmqEe4bIBP9pEZ4VG5H&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66VOazEoiMlVT5LyfIrJo00cvNuFdGVQSUgYSB1oL8UVePiNsSg_drQaAosTEALw_wcB&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://www.keyestudio.com/products/keyestudio-turbidity-sensor-v10-with-wires-compatible-with-arduino-for-water-testing</t>
+  </si>
+  <si>
+    <t>pH probe ENV 30</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/atlas-scientific/ENV-30-PH/16003028?gad_source=1&amp;gad_campaignid=20232005509&amp;gbraid=0AAAAADrbLliv6K8bW91YgzNqrt8ONo2QZ&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzpcO_PthZYBVBiTP7blHnIK4NnAfIL94wP-XbBh0unyx4OZTtFbw-hoC7p4QAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://atlas-scientific.com/probes/consumer-grade-ph-probe/?srsltid=AfmBOoog-hWZh-AcQq7td_rVXcdNzJnbRIhdNeb6Zga2Xtm4j7G4n8_-</t>
+  </si>
+  <si>
+    <t>TDS probe and conditioning circuit</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/184291373846?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=184291373846&amp;targetid=2299003535955&amp;device=c&amp;mktype=pla&amp;googleloc=9010352&amp;poi=&amp;campaignid=21214315381&amp;mkgroupid=161363866036&amp;rlsatarget=pla-2299003535955&amp;abcId=9407526&amp;merchantid=114832125&amp;gad_source=1&amp;gad_campaignid=21214315381&amp;gbraid=0AAAAAD_QDh-WxDW3V6tycLWe8cGWhVCet&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzg3Q1Yr5Qywajf85ozukT0eBrnuBw2qcSHroRC1sgV2p7BH7wwA-ZRoCue8QAvD_BwE</t>
+  </si>
+  <si>
+    <t>https://www.keyestudio.com/products/keyestudio-tds-meter-v10-board-module-water-meter-filter-measuring-water-quality-for-arduino-unor3</t>
+  </si>
+  <si>
+    <t>ds18b20 temperature sensor</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/224193475936?_skw=ds18b20&amp;itmmeta=01JWS9436Y9FERAQTKDM3HA2HJ&amp;hash=item3432f8f560:g:o3YAAOSwU~BfhkxY&amp;itmprp=enc%3AAQAKAAAA4FkggFvd1GGDu0w3yXCmi1eZVpkWHqnJ1CXCxYwe7hH8MTDd21uDFcQkxB6UmuFL1nzEvMyPnwrLbfpibrtSw6PJ6oEOTjHA%2BkjlTR3A1QaHWZf0kE2w%2FhydudbtDkwEMazkGGG3RxFLdxOnAGzZBTlCUEFESqTvAhNn%2Bjye4iJMlnnPGLOgNL40CCfjp7qUswlfOwv0yjnO%2Ft2tQ0Gx2dXExLjwUsFFwJLjU6q8t9vdK3%2FxrsrClja0ZOKas2024SmxIkA1w06CzLtlKOw3UkAT%2B%2FRsayZchEvbfvz6zTfc%7Ctkp%3ABFBM0rOQqeZl</t>
+  </si>
+  <si>
+    <t>https://www.dfrobot.com/product-689.html?gad_source=1&amp;gad_campaignid=22388643497&amp;gbraid=0AAAAADucPlAUqBsu3pP_X85ogWbbBBgBa&amp;gclid=Cj0KCQjwgvnCBhCqARIsADBLZoJ4ZCL5rKQ_98XjI9MZBlPRaBIgZRD5kPNfOK_USCuLZD6sqCQOP5UaArAjEALw_wcB</t>
+  </si>
+  <si>
+    <t>Male T connector for lipo</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/11864/6818769?gad_source=1&amp;gad_campaignid=20470400566&amp;gbraid=0AAAAADrbLliIHIRZTdCUnz0dgTjq27lO9&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzmI8CZGH_aIaTxCITd4vJTEk9RuU9JLQrgEuPZd__e3-SqyQUR2pSRoCVAQQAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://rcbattery.com/deans-style-t-connector-plug-male-side-5pcs-bag.html?gad_source=1&amp;gad_campaignid=12748770885&amp;gbraid=0AAAAACRJLSYkFmISdyi2KqVyCMKzbiA4R&amp;gclid=Cj0KCQjwgvnCBhCqARIsADBLZoK-nNIxyPzzUeK3H1UV2WeP_C8kJJqf35ExhChwl4khohXJRrsdQw8aAgtvEALw_wcB</t>
+  </si>
+  <si>
+    <t>15 pin female header 2.54 mm</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/SSW-115-01-F-S/7879494?gad_source=1&amp;gad_campaignid=17336967819&amp;gbraid=0AAAAADrbLlhPPMEXoJVxfpFdpEMhcu0YV&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66X6luvpzic7SpeQdTZEq5PP26iV0Bmu3w1zSQ-hOKFa4-GjmDPOJZMaAjkJEALw_wcB&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>PCB itself</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Net cost (USD)</t>
-  </si>
-  <si>
-    <t>Vendor 1</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_1206_3216Metric_Pad1.33x1.80mm_HandSolder</t>
-  </si>
-  <si>
-    <t>Resistor_SMD:R_1206_3216Metric_Pad1.30x1.75mm_HandSolder</t>
-  </si>
-  <si>
-    <t>SD card module</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>Arduino Nano</t>
-  </si>
-  <si>
-    <t>DS3231M</t>
-  </si>
-  <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>C1 0.1uF</t>
-  </si>
-  <si>
-    <t>R2 470ohm</t>
-  </si>
-  <si>
-    <t>3pin XH2.54 male connector</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-XH-A/1651046</t>
-  </si>
-  <si>
-    <t>R1 4.7K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/atlas-scientific/SRV-PH/16003016?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLlgG2JWtg72d3seRm9FjQrAou&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hznU8J98oZ-_7GD7xu8VgPNOpSYHGji59g_m7GB07rUIyNC8TPEMLYhoCYgIQAvD_BwE&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>Atlas pH conditioning circuit</t>
-  </si>
-  <si>
-    <t>ds18b20 temperature sensor</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/atlas-scientific/ENV-30-PH/16003028?gad_source=1&amp;gad_campaignid=20232005509&amp;gbraid=0AAAAADrbLliv6K8bW91YgzNqrt8ONo2QZ&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzpcO_PthZYBVBiTP7blHnIK4NnAfIL94wP-XbBh0unyx4OZTtFbw-hoC7p4QAvD_BwE&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>11.1V 3300mAH Lipo battery with T connector</t>
-  </si>
-  <si>
-    <t>Male T connector for lipo</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/nextgen-components/1206B104K500BD/15776047?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbRACYBmADgHYaQBdAgBwBcoQBlNgJwEsAdgHMQAXwLkADLACcCEMkjps%2BIqRBSAdGAAEAVoBiTVh0ggAqoP5sA8igCyONFgCuvHOIIBaeNEWomLgExJBkAGyUAKxRTGISFBqIaCxoiDaEvHFAA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/151033RS03000/4490003</t>
-  </si>
-  <si>
-    <t>15 pin female header 2.54 mm</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/11864/6818769?gad_source=1&amp;gad_campaignid=20470400566&amp;gbraid=0AAAAADrbLliIHIRZTdCUnz0dgTjq27lO9&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzmI8CZGH_aIaTxCITd4vJTEk9RuU9JLQrgEuPZd__e3-SqyQUR2pSRoCVAQQAvD_BwE&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/203852249807?_skw=SD+card+module+mini&amp;itmmeta=01JWS7YRSNYRE9JPQ1403XF1SB&amp;hash=item2f768a7acf:g:8QAAAOSwqApl32li&amp;itmprp=enc%3AAQAKAAAA8FkggFvd1GGDu0w3yXCmi1ebfwHB6lyAy277lL4U8xOIhySGOtjI0bRPLZxMt0nwv62q7s0aZTz%2Bx%2F%2B7upL3MEA0K%2Ft0uJJWEl1PUNUul0C2kuW4nvX2%2BRwcD%2FhFGnTe%2FYG8zjgNvBu3TQY4IOsJphAfcfdUNAqbhaX7gXxY59Lj77JBWoN7w1LfwWyMjbSTm6GobMFWOs8mooWe2dthd87YxK7TTSBoyUD9D2pQE62PZubKATklktRZLCgMHdh0lcqvJRpnSkfD1qwChuyoZk51pvBJMF9jfr6RlQAGIR8TsCDyF0H7ZR59sGEcWXB%2FYA%3D%3D%7Ctkp%3ABFBMhI37p-Zl</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/283932038203?_skw=arduino+nano&amp;itmmeta=01JWS81PY2BK5W7AA2FK7T4DBS&amp;hash=item421bab143b:g:LEAAAOSwdsFg2bYB&amp;itmprp=enc%3AAQAKAAAA8FkggFvd1GGDu0w3yXCmi1ctIY2mddW3r0Pkz46AoULbxKR%2BLiu5WOk62feEjacXqpl7sNYJ6oE5%2FIn8lx78btygJOm2GvQyRb5jvCpCuuGSTVPm9c07lGI3HNmnry6uXc%2FlnST9gzmAQ3twOlrPRg6L2z%2FrDEBP6lCqIj7RU29pAxunTYC5VGu28NSWzm60eskDXI6rlTmkwJlAt4v66kpFByyhd4g%2F6NwsaYSfKxSXG6ADA884XQD96VOVCodbJCGKGFFk37cKyzrKEAETZC68GmzoBgXTDf9gi8GNs2wRWd%2FEf3cay51rfG1Vttxmiw%3D%3D%7Ctkp%3ABk9SR5jvhqjmZQ</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/DS3231M-TRL/2402421</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/mpd-memory-protection-devices/BK-870/3829737</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR1206-JW-471ELF/3741054</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR1206-JW-472ELF/3785627</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/jauch-quartz/CR1025/16399048</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/184291373846?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=184291373846&amp;targetid=2299003535955&amp;device=c&amp;mktype=pla&amp;googleloc=9010352&amp;poi=&amp;campaignid=21214315381&amp;mkgroupid=161363866036&amp;rlsatarget=pla-2299003535955&amp;abcId=9407526&amp;merchantid=114832125&amp;gad_source=1&amp;gad_campaignid=21214315381&amp;gbraid=0AAAAAD_QDh-WxDW3V6tycLWe8cGWhVCet&amp;gclid=CjwKCAjwl_XBBhAUEiwAWK2hzg3Q1Yr5Qywajf85ozukT0eBrnuBw2qcSHroRC1sgV2p7BH7wwA-ZRoCue8QAvD_BwE</t>
-  </si>
-  <si>
-    <t>TDS probe and conditioning circuit</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/224193475936?_skw=ds18b20&amp;itmmeta=01JWS9436Y9FERAQTKDM3HA2HJ&amp;hash=item3432f8f560:g:o3YAAOSwU~BfhkxY&amp;itmprp=enc%3AAQAKAAAA4FkggFvd1GGDu0w3yXCmi1eZVpkWHqnJ1CXCxYwe7hH8MTDd21uDFcQkxB6UmuFL1nzEvMyPnwrLbfpibrtSw6PJ6oEOTjHA%2BkjlTR3A1QaHWZf0kE2w%2FhydudbtDkwEMazkGGG3RxFLdxOnAGzZBTlCUEFESqTvAhNn%2Bjye4iJMlnnPGLOgNL40CCfjp7qUswlfOwv0yjnO%2Ft2tQ0Gx2dXExLjwUsFFwJLjU6q8t9vdK3%2FxrsrClja0ZOKas2024SmxIkA1w06CzLtlKOw3UkAT%2B%2FRsayZchEvbfvz6zTfc%7Ctkp%3ABFBM0rOQqeZl</t>
-  </si>
-  <si>
-    <t>Vendor 2</t>
-  </si>
-  <si>
-    <t>Vendor 3</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/samtec-inc/SSW-115-01-F-S/7879494?gad_source=1&amp;gad_campaignid=17336967819&amp;gbraid=0AAAAADrbLlhPPMEXoJVxfpFdpEMhcu0YV&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66X6luvpzic7SpeQdTZEq5PP26iV0Bmu3w1zSQ-hOKFa4-GjmDPOJZMaAjkJEALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/c-k/OS102011MS2QN1/411602</t>
-  </si>
-  <si>
-    <t>SWITCH OS102011MS2QN1</t>
-  </si>
-  <si>
-    <t>LED 3.0mm</t>
-  </si>
-  <si>
-    <t>Coin cell battery CR-1025-ND</t>
-  </si>
-  <si>
-    <t>Coin cell Battery Holder BK-870</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/dfrobot/SEN0189/6588606?gad_source=1&amp;gad_campaignid=20243136172&amp;gbraid=0AAAAADrbLljucuLmqEe4bIBP9pEZ4VG5H&amp;gclid=Cj0KCQjwjJrCBhCXARIsAI5x66VOazEoiMlVT5LyfIrJo00cvNuFdGVQSUgYSB1oL8UVePiNsSg_drQaAosTEALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>Component spec / part number</t>
-  </si>
-  <si>
-    <t>PCB itself</t>
-  </si>
-  <si>
-    <t>https://oshpark.com/</t>
-  </si>
-  <si>
-    <t>https://www.keyestudio.com/products/keyestudio-turbidity-sensor-v10-with-wires-compatible-with-arduino-for-water-testing</t>
-  </si>
-  <si>
-    <t>Turbidity conditioning circuit and sensor</t>
-  </si>
-  <si>
-    <t>pH probe ENV 30</t>
-  </si>
-  <si>
-    <t>https://atlas-scientific.com/probes/consumer-grade-ph-probe/?srsltid=AfmBOoog-hWZh-AcQq7td_rVXcdNzJnbRIhdNeb6Zga2Xtm4j7G4n8_-</t>
-  </si>
-  <si>
-    <t>https://www.keyestudio.com/products/keyestudio-tds-meter-v10-board-module-water-meter-filter-measuring-water-quality-for-arduino-unor3</t>
-  </si>
-  <si>
     <t>Component</t>
   </si>
   <si>
     <t xml:space="preserve">Qty per sensor </t>
   </si>
   <si>
+    <t>Unit price (USD)</t>
+  </si>
+  <si>
+    <t>Net price (USD)</t>
+  </si>
+  <si>
     <t>vendor 1</t>
   </si>
   <si>
@@ -237,52 +270,40 @@
     <t>PVC union</t>
   </si>
   <si>
+    <t>https://www.grainger.com/product/22FL17?RIID=51819294775&amp;GID=729415832</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/pep/Apollo-2-in-x-2-in-PVC-Slip-Joint-x-Slip-Joint-Union-PVCU2/317901067?source=shoppingads&amp;locale=en-US&amp;pla&amp;utm_source=google&amp;utm_medium=vantage&amp;utm_campaign=52958&amp;utm_content=55246&amp;mtc=SHOPPING-RM-RMP-GGL-D26P-Multi-NA-APOLLO-NA-PMAX-NA-NA-MK897429001-52958-NBR-876-NA-VNT-FY25_Q1_Q4_THEMOSACKGROUPLLC_D26P_RM_ES_AON&amp;cm_mmc=SHOPPING-RM-RMP-GGL-D26P-Multi-NA-APOLLO-NA-PMAX-NA-NA-MK897429001-52958-NBR-876-NA-VNT-FY25_Q1_Q4_THEMOSACKGROUPLLC_D26P_RM_ES_AON-22224745817--&amp;gad_source=1&amp;gad_campaignid=22228588078&amp;gbraid=0AAAAAolLu989NOds_i5DS89vyDbOz8lsX&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD4wwYuEy7LBT_5YeRGvsomWTxN9uYDhqX3X0H-OD7fiaDyYfmt8F6IaAkX6EALw_wcB&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
     <t>Schedule 40 clear PVC pipe</t>
   </si>
   <si>
     <t>10 inches</t>
   </si>
   <si>
+    <t>https://www.grainger.com/product/1AAZ8?gucid=N:N:PS:Paid:GGL:CSM-2295:Y8ZQJW:20500801:APZ_1&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=21375667808&amp;gclid=EAIaIQobChMI5eGkh7jsjQMV0kf_AR21aSMcEAQYASABEgKqH_D_BwE</t>
+  </si>
+  <si>
     <t>Schedule 40 socket cap</t>
   </si>
   <si>
+    <t>https://www.grainger.com/product/22FJ37?RIID=51819294775&amp;GID=729415832</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/pep/Charlotte-Pipe-2-in-PVC-Socket-Schedule-40-Pressure-Cap-PVC021161600HD/203811678?source=shoppingads&amp;locale=en-US&amp;pla&amp;mtc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PLALIA-NA-NA-NA-NA-NBR-NA-NA-NEW-_PLATEST&amp;cm_mmc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PLALIA-NA-NA-NA-NA-NBR-NA-NA-NEW-_PLATEST-22111492781-173962209835-331272778036&amp;gad_source=1&amp;gad_campaignid=22111492781&amp;gbraid=0AAAAADq61UeV86D9Cm_YSFHZ_xQoepPWR&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7hsSItt8-j7uHZGoH9ZOHc9dwlTetTnvM1YPIH3krowDG1cA4a5pgaAihuEALw_wcB&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/pep/Charlotte-Pipe-2-in-OD-PVC-Test-Cap-Fitting-PVC-00132-0800HD/203947220?source=shoppingads&amp;locale=en-US&amp;pla&amp;mtc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PMAX-NA-NA-NA-NA-NBR-NA-NA-NEW-_PMAXTEST&amp;cm_mmc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PMAX-NA-NA-NA-NA-NBR-NA-NA-NEW-_PMAXTEST-17697557984--&amp;gad_source=1&amp;gad_campaignid=17687574624&amp;gbraid=0AAAAADq61Ufi2up4If7IM8ksnlizOw_kh&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD49Pa9Dm1h-kkEkDeErgMj2io-t9JfRe__p697sfPoJ_qcdwpJCxWMaAjS6EALw_wcB&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
     <t>2 part epoxy</t>
   </si>
   <si>
-    <t>Net price (USD)</t>
-  </si>
-  <si>
-    <t>Unit price (USD)</t>
+    <t>1 pack</t>
   </si>
   <si>
     <t>https://www.grainger.com/product/25F529?gucid=N:N:PS:Paid:GGL:CSM-2295:7Q8R4W:20500801:APZ_1&amp;gad_source=1&amp;gad_campaignid=21369464154&amp;gclid=CjwKCAjwr5_CBhBlEiwAzfwYuFQJQF4xih2fA0vbI8pFLV_pGSsb1GvVdYQqLORI5ApakqFVLNHuxxoCPr8QAvD_BwE&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>1 pack</t>
-  </si>
-  <si>
-    <t>https://www.grainger.com/product/1AAZ8?gucid=N:N:PS:Paid:GGL:CSM-2295:Y8ZQJW:20500801:APZ_1&amp;gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=21375667808&amp;gclid=EAIaIQobChMI5eGkh7jsjQMV0kf_AR21aSMcEAQYASABEgKqH_D_BwE</t>
-  </si>
-  <si>
-    <t>https://www.homedepot.com/pep/Apollo-2-in-x-2-in-PVC-Slip-Joint-x-Slip-Joint-Union-PVCU2/317901067?source=shoppingads&amp;locale=en-US&amp;pla&amp;utm_source=google&amp;utm_medium=vantage&amp;utm_campaign=52958&amp;utm_content=55246&amp;mtc=SHOPPING-RM-RMP-GGL-D26P-Multi-NA-APOLLO-NA-PMAX-NA-NA-MK897429001-52958-NBR-876-NA-VNT-FY25_Q1_Q4_THEMOSACKGROUPLLC_D26P_RM_ES_AON&amp;cm_mmc=SHOPPING-RM-RMP-GGL-D26P-Multi-NA-APOLLO-NA-PMAX-NA-NA-MK897429001-52958-NBR-876-NA-VNT-FY25_Q1_Q4_THEMOSACKGROUPLLC_D26P_RM_ES_AON-22224745817--&amp;gad_source=1&amp;gad_campaignid=22228588078&amp;gbraid=0AAAAAolLu989NOds_i5DS89vyDbOz8lsX&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD4wwYuEy7LBT_5YeRGvsomWTxN9uYDhqX3X0H-OD7fiaDyYfmt8F6IaAkX6EALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>https://www.homedepot.com/pep/Charlotte-Pipe-2-in-PVC-Socket-Schedule-40-Pressure-Cap-PVC021161600HD/203811678?source=shoppingads&amp;locale=en-US&amp;pla&amp;mtc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PLALIA-NA-NA-NA-NA-NBR-NA-NA-NEW-_PLATEST&amp;cm_mmc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PLALIA-NA-NA-NA-NA-NBR-NA-NA-NEW-_PLATEST-22111492781-173962209835-331272778036&amp;gad_source=1&amp;gad_campaignid=22111492781&amp;gbraid=0AAAAADq61UeV86D9Cm_YSFHZ_xQoepPWR&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7hsSItt8-j7uHZGoH9ZOHc9dwlTetTnvM1YPIH3krowDG1cA4a5pgaAihuEALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>https://www.homedepot.com/pep/Charlotte-Pipe-2-in-OD-PVC-Test-Cap-Fitting-PVC-00132-0800HD/203947220?source=shoppingads&amp;locale=en-US&amp;pla&amp;mtc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PMAX-NA-NA-NA-NA-NBR-NA-NA-NEW-_PMAXTEST&amp;cm_mmc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PMAX-NA-NA-NA-NA-NBR-NA-NA-NEW-_PMAXTEST-17697557984--&amp;gad_source=1&amp;gad_campaignid=17687574624&amp;gbraid=0AAAAADq61Ufi2up4If7IM8ksnlizOw_kh&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD49Pa9Dm1h-kkEkDeErgMj2io-t9JfRe__p697sfPoJ_qcdwpJCxWMaAjS6EALw_wcB&amp;gclsrc=aw.ds</t>
-  </si>
-  <si>
-    <t>https://www.grainger.com/product/22FJ37?RIID=51819294775&amp;GID=729415832</t>
-  </si>
-  <si>
-    <t>https://www.grainger.com/product/22FL17?RIID=51819294775&amp;GID=729415832</t>
-  </si>
-  <si>
-    <t>https://us.ovonicshop.com/products/2-ovonic-3000mah-3s-50c-lipo-battery-11-1v-long-with-t-plug-for-aircraft?variant=49495640736024&amp;country=US&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;gad_source=1&amp;gad_campaignid=22231059484&amp;gbraid=0AAAAADH9voLksvZtdQfP_qv6g9D5uP4vz&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7wVC7linJpS4qPBFEeagS1am8YjtEL9eHuExf6EBj_sSKmwI5S25AaAmK1EALw_wcB</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/184508325888?chn=ps&amp;_trkparms=ispr%3D1&amp;amdata=enc%3A1ylpS771GTUqS6YST7-apLg15&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=184508325888&amp;targetid=2321110924221&amp;device=c&amp;mktype=pla&amp;googleloc=9010433&amp;poi=&amp;campaignid=21400684010&amp;mkgroupid=173029508068&amp;rlsatarget=aud-1317046432738:pla-2321110924221&amp;abcId=9448486&amp;merchantid=118955226&amp;gad_source=1&amp;gad_campaignid=21400684010&amp;gbraid=0AAAAAD_QDh99tBHCSfvM5L2BJj0mpS-rS&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7LhNJPcz_yB99-iNQOigF1uTLSpT72VMRZDt4bpaZcj-4-2mtZYDUaAlYNEALw_wcB</t>
   </si>
 </sst>
 </file>
@@ -988,10 +1009,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1313,221 +1330,267 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF72E9-9057-43B3-9849-7848ED564DB8}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="2" width="61.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="61.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" customWidth="1"/>
     <col min="5" max="5" width="15.81640625" customWidth="1"/>
     <col min="6" max="6" width="86" customWidth="1"/>
-    <col min="7" max="8" width="46.6328125" customWidth="1"/>
+    <col min="7" max="8" width="46.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.11</v>
+      </c>
       <c r="F2" s="10" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="8">
+        <v>0.71</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.71</v>
+      </c>
       <c r="F3" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.16</v>
+      </c>
       <c r="F4" s="10" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="8">
+        <v>1.69</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1.69</v>
+      </c>
       <c r="F5" s="10" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="8">
+        <v>3.67</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3.67</v>
+      </c>
       <c r="F6" s="10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="8">
+        <v>10.98</v>
+      </c>
+      <c r="E7" s="8">
+        <v>10.98</v>
+      </c>
       <c r="F7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C8" s="8">
         <v>1</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="F8" s="10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C9" s="8">
         <v>1</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.13</v>
+      </c>
       <c r="F9" s="10" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.1</v>
+      </c>
       <c r="F10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.1</v>
+      </c>
       <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
@@ -1536,188 +1599,234 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="8">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1.0900000000000001</v>
+      </c>
       <c r="F12" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" ht="203" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C13" s="8">
         <v>1</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="8">
+        <v>46.72</v>
+      </c>
+      <c r="E13" s="8">
+        <v>46.72</v>
+      </c>
       <c r="F13" s="10" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="11"/>
+        <v>45</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="8">
+        <v>26.11</v>
+      </c>
+      <c r="E14" s="8">
+        <v>26.11</v>
+      </c>
       <c r="F14" s="10" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="8">
+        <v>9.9</v>
+      </c>
+      <c r="E15" s="8">
+        <v>9.9</v>
+      </c>
       <c r="F15" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="8">
+        <v>49.99</v>
+      </c>
+      <c r="E16" s="8">
+        <v>49.99</v>
+      </c>
       <c r="F16" s="10" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C17" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="8">
+        <v>19.95</v>
+      </c>
+      <c r="E17" s="8">
+        <v>19.95</v>
+      </c>
       <c r="F17" s="10" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C18" s="8">
         <v>1</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="8">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2.5499999999999998</v>
+      </c>
       <c r="F18" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C19" s="8">
         <v>1</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="D19" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1.25</v>
+      </c>
       <c r="F19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="10"/>
+        <v>62</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C20" s="8">
         <v>2</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E20" s="8">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="F20" s="10" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C21" s="8">
         <v>1</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="8">
+        <v>8</v>
+      </c>
+      <c r="E21" s="8">
+        <v>8</v>
+      </c>
       <c r="F21" s="10" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -1726,11 +1835,11 @@
       <c r="A22" s="12"/>
       <c r="C22" s="9"/>
       <c r="D22" s="13" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="E22" s="14">
-        <f>SUM(E2:E20)</f>
-        <v>0</v>
+        <f>SUM(E3:E21)</f>
+        <v>188.08</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="12"/>
@@ -1763,9 +1872,15 @@
     <hyperlink ref="G17" r:id="rId23" xr:uid="{4C6031E9-5DB5-420D-A786-DB2505BC5E3F}"/>
     <hyperlink ref="F13" r:id="rId24" display="https://us.ovonicshop.com/products/2-ovonic-3000mah-3s-50c-lipo-battery-11-1v-long-with-t-plug-for-aircraft?variant=49495640736024&amp;country=US&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;gad_source=1&amp;gad_campaignid=22231059484&amp;gbraid=0AAAAADH9voLksvZtdQfP_qv6g9D5uP4vz&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7wVC7linJpS4qPBFEeagS1am8YjtEL9eHuExf6EBj_sSKmwI5S25AaAmK1EALw_wcB" xr:uid="{92AF7484-CF48-43A5-87AC-D1D1E4726FFC}"/>
     <hyperlink ref="G13" r:id="rId25" display="https://www.ebay.com/itm/184508325888?chn=ps&amp;_trkparms=ispr%3D1&amp;amdata=enc%3A1ylpS771GTUqS6YST7-apLg15&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=184508325888&amp;targetid=2321110924221&amp;device=c&amp;mktype=pla&amp;googleloc=9010433&amp;poi=&amp;campaignid=21400684010&amp;mkgroupid=173029508068&amp;rlsatarget=aud-1317046432738:pla-2321110924221&amp;abcId=9448486&amp;merchantid=118955226&amp;gad_source=1&amp;gad_campaignid=21400684010&amp;gbraid=0AAAAAD_QDh99tBHCSfvM5L2BJj0mpS-rS&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7LhNJPcz_yB99-iNQOigF1uTLSpT72VMRZDt4bpaZcj-4-2mtZYDUaAlYNEALw_wcB" xr:uid="{3CB92383-C82A-4483-8BB2-4316CC09D92E}"/>
+    <hyperlink ref="H13" r:id="rId26" display="https://www.motionrc.com/products/admiral-3300mah-3s-11-1v-30c-lipo-battery-with-t-connector-epr33003?variant=19047011142&amp;country=US&amp;currency=USD&amp;utm_medium=product_sync&amp;utm_source=google&amp;utm_content=sag_organic&amp;utm_campaign=sag_organic&amp;gad_source=1&amp;gad_campaignid=15448361688&amp;gbraid=0AAAAADrr98ZD1fBrj_NSKbi2hqFZgUrfk&amp;gclid=Cj0KCQjwgvnCBhCqARIsADBLZoIjaMcUy2YxUOv0QnymhbqBDrWMvbmN8Xkj10xanB3EhIRIsKdz-QAaAkkxEALw_wcB" xr:uid="{33A0557F-BAF8-45FF-A06A-9B35F82DC323}"/>
+    <hyperlink ref="G3" r:id="rId27" display="https://www.mouser.com/ProductDetail/CK/OS102011MS2QN1?qs=WtljUlYws5RvQ1hEv876nQ%3D%3D&amp;mgh=1&amp;utm_id=22174357374&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_marketing_tactic=amercorp&amp;gad_source=1&amp;gad_campaignid=22295195434&amp;gbraid=0AAAAADn_wf37NcPripZZCoy9AiD-OvAcG&amp;gclid=Cj0KCQjwgvnCBhCqARIsADBLZoKyGA5ClHUZR7eCJ8ET8sUhF8oXtsBAC19VweIc1X0k5wSmKxZJZCcaAhNFEALw_wcB " xr:uid="{925E73F0-7493-4F10-B879-D8FE7A9712D3}"/>
+    <hyperlink ref="H3" r:id="rId28" xr:uid="{9966B871-4776-420A-8EA7-07123C5518BF}"/>
+    <hyperlink ref="G7" r:id="rId29" display="https://www.mouser.com/ProductDetail/Analog-Devices-Maxim-Integrated/DS3231M+TRL?qs=Bakm8ERcljq5PBzSwLfmgg%3D%3D&amp;utm_id=22337522785&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_marketing_tactic=amercorp&amp;gad_source=1&amp;gad_campaignid=22327353774&amp;gbraid=0AAAAADn_wf3tXOv7c9Y4wq2-Yvx_HD5I2&amp;gclid=Cj0KCQjwgvnCBhCqARIsADBLZoJwmYFO86Wu0iC_hUhm8R9ynjb29I-YIssyZ4USDWwZGmZXPXlNSLQaAlaREALw_wcB" xr:uid="{CBA3015C-15AD-4E96-9E48-B76639C15CC9}"/>
+    <hyperlink ref="G18" r:id="rId30" xr:uid="{D9663DC4-76A3-45BB-9383-32E9FD3E3482}"/>
+    <hyperlink ref="G19" r:id="rId31" xr:uid="{05851BE9-43B5-4810-BCBB-114F8BF3D559}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -1773,14 +1888,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC825CFC-606A-4EB1-BF18-3BEFDFC7363F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="E2:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.36328125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" style="22" customWidth="1"/>
     <col min="3" max="4" width="18.81640625" style="18" customWidth="1"/>
     <col min="5" max="5" width="65.453125" style="18" customWidth="1"/>
     <col min="6" max="7" width="58" style="18" customWidth="1"/>
@@ -1789,98 +1904,115 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>71</v>
-      </c>
       <c r="E1" s="17" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B2" s="19">
         <v>1</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="23">
+        <v>19.559999999999999</v>
+      </c>
+      <c r="D2" s="23">
+        <v>19.559999999999999</v>
+      </c>
       <c r="E2" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+        <v>80</v>
+      </c>
+      <c r="C3" s="19">
+        <v>69.69</v>
+      </c>
+      <c r="D3" s="19">
+        <v>7.26</v>
+      </c>
       <c r="E3" s="5" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="23">
+        <v>1.47</v>
+      </c>
+      <c r="D4" s="23">
+        <v>1.47</v>
+      </c>
       <c r="E4" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C5" s="23">
         <v>47.86</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="23">
+        <v>47.86</v>
+      </c>
       <c r="E5" s="5" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
+      <c r="D6" s="25">
+        <f>SUM(D2:D5)</f>
+        <v>76.150000000000006</v>
+      </c>
       <c r="E6" s="20"/>
     </row>
   </sheetData>
@@ -1888,6 +2020,9 @@
     <hyperlink ref="E5" r:id="rId1" xr:uid="{BB44769E-9C2A-4FEF-A4D5-DBD7D743C569}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{B6F53024-3E40-4537-A6CB-957ECEAB506D}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{C7E53F22-BC80-4F02-BB31-9E92055C075F}"/>
+    <hyperlink ref="F2" r:id="rId4" display="https://www.homedepot.com/pep/Apollo-2-in-x-2-in-PVC-Slip-Joint-x-Slip-Joint-Union-PVCU2/317901067?source=shoppingads&amp;locale=en-US&amp;pla&amp;utm_source=google&amp;utm_medium=vantage&amp;utm_campaign=52958&amp;utm_content=55246&amp;mtc=SHOPPING-RM-RMP-GGL-D26P-Multi-NA-APOLLO-NA-PMAX-NA-NA-MK897429001-52958-NBR-876-NA-VNT-FY25_Q1_Q4_THEMOSACKGROUPLLC_D26P_RM_ES_AON&amp;cm_mmc=SHOPPING-RM-RMP-GGL-D26P-Multi-NA-APOLLO-NA-PMAX-NA-NA-MK897429001-52958-NBR-876-NA-VNT-FY25_Q1_Q4_THEMOSACKGROUPLLC_D26P_RM_ES_AON-22224745817--&amp;gad_source=1&amp;gad_campaignid=22228588078&amp;gbraid=0AAAAAolLu989NOds_i5DS89vyDbOz8lsX&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD4wwYuEy7LBT_5YeRGvsomWTxN9uYDhqX3X0H-OD7fiaDyYfmt8F6IaAkX6EALw_wcB&amp;gclsrc=aw.ds" xr:uid="{EAC7F3EE-311A-448F-ADCF-A6A93E974701}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{2632D8A7-1920-48A2-8E3B-00409A6C33EC}"/>
+    <hyperlink ref="F4" r:id="rId6" display="https://www.homedepot.com/pep/Charlotte-Pipe-2-in-PVC-Socket-Schedule-40-Pressure-Cap-PVC021161600HD/203811678?source=shoppingads&amp;locale=en-US&amp;pla&amp;mtc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PLALIA-NA-NA-NA-NA-NBR-NA-NA-NEW-_PLATEST&amp;cm_mmc=SHOPPING-BF-CDP-GGL-D26P-026_001_PIPE_FITTING-NA-NA-NA-PLALIA-NA-NA-NA-NA-NBR-NA-NA-NEW-_PLATEST-22111492781-173962209835-331272778036&amp;gad_source=1&amp;gad_campaignid=22111492781&amp;gbraid=0AAAAADq61UeV86D9Cm_YSFHZ_xQoepPWR&amp;gclid=Cj0KCQjwmK_CBhCEARIsAMKwcD7hsSItt8-j7uHZGoH9ZOHc9dwlTetTnvM1YPIH3krowDG1cA4a5pgaAihuEALw_wcB&amp;gclsrc=aw.ds" xr:uid="{567967C8-8E6D-4379-95E2-13CF4EF3C1C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>